<commit_message>
2024.07.06 add: 6.17-7.05报告.md, 英才计划中期总结.pptx
</commit_message>
<xml_diff>
--- a/学习计划与资料/学习计划.xlsx
+++ b/学习计划与资料/学习计划.xlsx
@@ -698,7 +698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="84" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="111" customFormat="1" s="1">
       <c r="A9" s="2">
         <f>A8+7</f>
         <v>25569.333333333332</v>
@@ -717,7 +717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="57.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="81" customFormat="1" s="1">
       <c r="A10" s="2">
         <f>A9+7</f>
         <v>25569.333333333332</v>
@@ -736,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="31.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A11" s="2">
         <f>A10+7</f>
         <v>25569.333333333332</v>
@@ -755,7 +755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="31.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="36" customFormat="1" s="1">
       <c r="A12" s="2">
         <f>A11+7</f>
         <v>25569.333333333332</v>
@@ -774,7 +774,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="84" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="111" customFormat="1" s="1">
       <c r="A13" s="2">
         <f>A12+7</f>
         <v>25569.333333333332</v>

</xml_diff>